<commit_message>
Added bGigeiCast files to be implemented
</commit_message>
<xml_diff>
--- a/designs/hardware/ESP32 nGeigieNano WiFi/BOM bGeigieCast.xlsx
+++ b/designs/hardware/ESP32 nGeigieNano WiFi/BOM bGeigieCast.xlsx
@@ -160,6 +160,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -351,17 +352,18 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="35.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.64"/>
   </cols>

</xml_diff>